<commit_message>
Deploying to gh-pages from  @ bc22c8d72bdacadfa5fdd16e9bec342e9d9d47a8 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/9.b.1.xlsx
+++ b/en/downloads/data-excel/9.b.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\korozbaeva\Desktop\ПоказателиЦУР для Платформы\Глобальные показатели ЦУР\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\korozbaeva\Desktop\Показатели ЦУР для Платформы\Глобальные показатели ЦУР\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -564,16 +564,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="38.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="51" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="51" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>8</v>
       </c>
@@ -594,7 +596,7 @@
       <c r="L1" s="15"/>
       <c r="M1" s="15"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>4</v>
       </c>
@@ -615,7 +617,7 @@
       <c r="L2" s="16"/>
       <c r="M2" s="16"/>
     </row>
-    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -630,7 +632,7 @@
       <c r="L3" s="16"/>
       <c r="M3" s="16"/>
     </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -664,8 +666,11 @@
       <c r="M4" s="8">
         <v>2019</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N4" s="8">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>10</v>
       </c>
@@ -714,8 +719,11 @@
       <c r="M5" s="17">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="N5" s="17">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>

</xml_diff>